<commit_message>
Fix +1 bug, where first style number was 165 instead of 164, if there was a built-in style reference with a number from 0..163 (without format code, because it is built-in number format)
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/AutoFilter/DateTimeGroupAutoFilter.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/AutoFilter/DateTimeGroupAutoFilter.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t>Dates</x:t>
   </x:si>
@@ -27,7 +27,7 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="165" formatCode="d MMMM yyyy"/>
+    <x:numFmt numFmtId="164" formatCode="d MMMM yyyy"/>
   </x:numFmts>
   <x:fonts count="1">
     <x:font>
@@ -69,7 +69,7 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -78,7 +78,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>